<commit_message>
Teste de novo commit
</commit_message>
<xml_diff>
--- a/curso 2 - procv.xlsx
+++ b/curso 2 - procv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GabrielaMoreira\Downloads\excel-procv-material-inicial\excel-procv-material-inicial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GabrielaMoreira\Documents\5_ALURA\Formacao_excel_VBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFA3280-4E9A-415C-857A-9A6CA842A695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B39CDDA-93A3-48A8-AF31-CB6C39A9ED59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7995" firstSheet="2" activeTab="3" xr2:uid="{C1B61AA5-C757-4C13-B5B2-E36863709022}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="1" xr2:uid="{C1B61AA5-C757-4C13-B5B2-E36863709022}"/>
   </bookViews>
   <sheets>
     <sheet name="Produtos Infantis" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +297,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -891,42 +898,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
@@ -966,13 +937,7 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="10" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1003,6 +968,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1015,6 +1010,18 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hiperlink" xfId="3" builtinId="8"/>
@@ -1022,7 +1029,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -1040,16 +1047,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC1C1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6269,14 +6266,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="82"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -8421,14 +8418,14 @@
         <v>89.9</v>
       </c>
       <c r="D99" s="17">
-        <f t="shared" ref="D99:D130" si="6">C99*$C$124</f>
+        <f t="shared" ref="D99:D122" si="6">C99*$C$124</f>
         <v>8.99</v>
       </c>
       <c r="E99" s="19">
         <v>4</v>
       </c>
       <c r="F99" s="17">
-        <f t="shared" ref="F99:F130" si="7">(C99-D99)*E99</f>
+        <f t="shared" ref="F99:F122" si="7">(C99-D99)*E99</f>
         <v>323.64000000000004</v>
       </c>
     </row>
@@ -8962,12 +8959,12 @@
       <c r="B124" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C124" s="50">
+      <c r="C124" s="83">
         <v>0.1</v>
       </c>
-      <c r="D124" s="51"/>
-      <c r="E124" s="51"/>
-      <c r="F124" s="52"/>
+      <c r="D124" s="84"/>
+      <c r="E124" s="84"/>
+      <c r="F124" s="85"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F122">
@@ -8986,8 +8983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF919602-C1FD-4070-AC2D-96214F3A5DDA}">
   <dimension ref="A1:V14"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8996,31 +8993,31 @@
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="46"/>
       <c r="B1" s="46"/>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="54"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+      <c r="U1" s="96"/>
+      <c r="V1" s="97"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="46"/>
@@ -9087,7 +9084,7 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="87" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="45" t="s">
@@ -9155,7 +9152,7 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
+      <c r="A4" s="86"/>
       <c r="B4" s="40" t="s">
         <v>28</v>
       </c>
@@ -9221,7 +9218,7 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="86" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="40" t="s">
@@ -9289,7 +9286,7 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
+      <c r="A6" s="86"/>
       <c r="B6" s="40" t="s">
         <v>28</v>
       </c>
@@ -9355,7 +9352,7 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="86" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="40" t="s">
@@ -9423,7 +9420,7 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
+      <c r="A8" s="86"/>
       <c r="B8" s="40" t="s">
         <v>28</v>
       </c>
@@ -9489,7 +9486,7 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="86" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="40" t="s">
@@ -9557,7 +9554,7 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+      <c r="A10" s="86"/>
       <c r="B10" s="40" t="s">
         <v>28</v>
       </c>
@@ -9623,7 +9620,7 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="86" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="40" t="s">
@@ -9691,7 +9688,7 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
+      <c r="A12" s="86"/>
       <c r="B12" s="40" t="s">
         <v>28</v>
       </c>
@@ -9757,7 +9754,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="86" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="40" t="s">
@@ -9825,7 +9822,7 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
+      <c r="A14" s="86"/>
       <c r="B14" s="40" t="s">
         <v>28</v>
       </c>
@@ -9901,6 +9898,7 @@
     <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9914,352 +9912,352 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="3.42578125" style="59" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="59" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" style="59" customWidth="1"/>
-    <col min="6" max="9" width="3.7109375" style="59" customWidth="1"/>
-    <col min="10" max="10" width="10" style="59" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="59" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="59" customWidth="1"/>
-    <col min="13" max="13" width="3.42578125" style="59" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="59"/>
+    <col min="1" max="3" width="3.42578125" style="47" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="47" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" style="47" customWidth="1"/>
+    <col min="6" max="9" width="3.7109375" style="47" customWidth="1"/>
+    <col min="10" max="10" width="10" style="47" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="47" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="47" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" style="47" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="61"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="63"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="63"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="51"/>
     </row>
     <row r="4" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="60"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="80" t="s">
+      <c r="B4" s="48"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="67"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="80" t="s">
+      <c r="E4" s="89"/>
+      <c r="F4" s="55"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="67"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="55"/>
     </row>
     <row r="5" spans="2:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="60"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="67"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="67"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="55"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="60"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="73" t="s">
+      <c r="B6" s="48"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="79" t="s">
+      <c r="E6" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="67"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="67"/>
+      <c r="F6" s="55"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
     </row>
     <row r="7" spans="2:13" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="60"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="67"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="67"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="55"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="55"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="60"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="73" t="s">
+      <c r="B8" s="48"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="72">
+      <c r="E8" s="60">
         <v>21</v>
       </c>
-      <c r="F8" s="67"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="82" t="s">
+      <c r="F8" s="55"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="82"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="67"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="55"/>
     </row>
     <row r="9" spans="2:13" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="60"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="67"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="88">
+      <c r="B9" s="48"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="74">
         <v>0</v>
       </c>
-      <c r="L9" s="89">
+      <c r="L9" s="75">
         <v>0</v>
       </c>
-      <c r="M9" s="67"/>
+      <c r="M9" s="55"/>
     </row>
     <row r="10" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="60"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="73" t="s">
+      <c r="B10" s="48"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="72">
+      <c r="E10" s="60">
         <v>3</v>
       </c>
-      <c r="F10" s="67"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="66" t="s">
+      <c r="F10" s="55"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="86">
+      <c r="K10" s="72">
         <v>150</v>
       </c>
-      <c r="L10" s="87">
+      <c r="L10" s="73">
         <v>0.08</v>
       </c>
-      <c r="M10" s="67"/>
+      <c r="M10" s="55"/>
     </row>
     <row r="11" spans="2:13" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="60"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="67"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="85"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="67"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="55"/>
     </row>
     <row r="12" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="60"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="73" t="s">
+      <c r="B12" s="48"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="83">
+      <c r="E12" s="69">
         <f>IF(VLOOKUP(E10,K15:L18,2,TRUE) &gt; VLOOKUP(E16,K9:L12,2,TRUE), VLOOKUP(E10,K15:L18,2,TRUE), VLOOKUP(E16,K9:L12,2,TRUE))</f>
         <v>0.08</v>
       </c>
-      <c r="F12" s="67"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="66" t="s">
+      <c r="F12" s="55"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="K12" s="86">
+      <c r="K12" s="72">
         <v>300</v>
       </c>
-      <c r="L12" s="87">
+      <c r="L12" s="73">
         <v>0.15</v>
       </c>
-      <c r="M12" s="67"/>
+      <c r="M12" s="55"/>
     </row>
     <row r="13" spans="2:13" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="60"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="67"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="67"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="55"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="60"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="73" t="s">
+      <c r="B14" s="48"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="76">
+      <c r="E14" s="64">
         <f>IFERROR(HLOOKUP(E8,DadosT,MATCH(E6,Titulos,0),FALSE),"Produto não encontrado!")</f>
         <v>12</v>
       </c>
-      <c r="F14" s="67"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="82" t="s">
+      <c r="F14" s="55"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="82"/>
-      <c r="L14" s="82"/>
-      <c r="M14" s="67"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="55"/>
     </row>
     <row r="15" spans="2:13" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="60"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="67"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="88">
+      <c r="B15" s="48"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="55"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="74">
         <v>0</v>
       </c>
-      <c r="L15" s="89">
+      <c r="L15" s="75">
         <v>0</v>
       </c>
-      <c r="M15" s="67"/>
+      <c r="M15" s="55"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="60"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="73" t="s">
+      <c r="B16" s="48"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="77">
+      <c r="E16" s="65">
         <f>IFERROR(INDEX('Produtos Infantis por Coluna'!C3:V14,D21,E21)*E10,"Produto não encontrado!")</f>
         <v>239.39999999999998</v>
       </c>
-      <c r="F16" s="67"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="64"/>
-      <c r="J16" s="73" t="s">
+      <c r="F16" s="55"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="K16" s="85">
+      <c r="K16" s="71">
         <v>2</v>
       </c>
-      <c r="L16" s="81">
+      <c r="L16" s="68">
         <v>0.05</v>
       </c>
-      <c r="M16" s="67"/>
+      <c r="M16" s="55"/>
     </row>
     <row r="17" spans="2:13" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="60"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="67"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="85"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="67"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="55"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="55"/>
     </row>
     <row r="18" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="60"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="78" t="str">
+      <c r="B18" s="48"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="66" t="str">
         <f>_xlfn.IFS(E14=0,"Produto Esgotado!", E14&lt;=4, "Estoque Baixo!", TRUE, "")</f>
         <v/>
       </c>
-      <c r="F18" s="67"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="66" t="s">
+      <c r="F18" s="55"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="K18" s="85">
+      <c r="K18" s="71">
         <v>5</v>
       </c>
-      <c r="L18" s="81">
+      <c r="L18" s="68">
         <v>0.09</v>
       </c>
-      <c r="M18" s="67"/>
+      <c r="M18" s="55"/>
     </row>
     <row r="19" spans="2:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="60"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="67"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="64"/>
-      <c r="J19" s="66"/>
-      <c r="K19" s="85"/>
-      <c r="L19" s="91"/>
-      <c r="M19" s="67"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="55"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="77"/>
+      <c r="M19" s="55"/>
     </row>
     <row r="20" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="60"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="92" t="s">
+      <c r="B20" s="48"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="66"/>
-      <c r="F20" s="67"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="66"/>
-      <c r="K20" s="66"/>
-      <c r="L20" s="66"/>
-      <c r="M20" s="67"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="55"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="55"/>
     </row>
     <row r="21" spans="2:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="60"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="74">
+      <c r="B21" s="48"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="62">
         <f>MATCH(E6,'Produtos Infantis por Coluna'!A3:A14,0)</f>
         <v>1</v>
       </c>
-      <c r="E21" s="74">
+      <c r="E21" s="62">
         <f>MATCH(E8,'Produtos Infantis por Coluna'!C2:V2,0)</f>
         <v>5</v>
       </c>
-      <c r="F21" s="70"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="70"/>
+      <c r="F21" s="58"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="58"/>
     </row>
     <row r="22" spans="2:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="60"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="60"/>
-      <c r="L22" s="60"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -10270,12 +10268,12 @@
     <mergeCell ref="D4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>E14&lt;=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10296,229 +10294,229 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1BA7B8-F3DB-4ED4-A0ED-2E319E512525}">
   <dimension ref="B1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="3.42578125" style="59" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="59" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" style="59" customWidth="1"/>
-    <col min="6" max="7" width="3.7109375" style="59" customWidth="1"/>
-    <col min="8" max="9" width="3.42578125" style="59" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" style="59" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.42578125" style="59" customWidth="1"/>
-    <col min="12" max="12" width="3.7109375" style="59" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="59"/>
+    <col min="1" max="3" width="3.42578125" style="47" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="47" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" style="47" customWidth="1"/>
+    <col min="6" max="7" width="3.7109375" style="47" customWidth="1"/>
+    <col min="8" max="9" width="3.42578125" style="47" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" style="47" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" style="47" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="61"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="63"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="63"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="51"/>
     </row>
     <row r="4" spans="2:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="60"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="80" t="s">
+      <c r="B4" s="48"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="67"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="80" t="s">
+      <c r="E4" s="89"/>
+      <c r="F4" s="55"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="80"/>
-      <c r="L4" s="67"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="55"/>
     </row>
     <row r="5" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="60"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="67"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="67"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="55"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="60"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="73" t="s">
+      <c r="B6" s="48"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="90" t="str">
+      <c r="E6" s="76" t="str">
         <f>'Procura em Estoque'!E6</f>
         <v>Tênis Infantil Atitas Azul</v>
       </c>
-      <c r="F6" s="67"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="73" t="s">
+      <c r="F6" s="55"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="90" t="b">
+      <c r="K6" s="76" t="b">
         <v>1</v>
       </c>
-      <c r="L6" s="67"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="2:12" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="60"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="67"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="67"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="55"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="55"/>
     </row>
     <row r="8" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="60"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="73" t="s">
+      <c r="B8" s="48"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="75">
+      <c r="E8" s="63">
         <f>'Procura em Estoque'!E10</f>
         <v>3</v>
       </c>
-      <c r="F8" s="67"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="73" t="s">
+      <c r="F8" s="55"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="75" t="b">
+      <c r="K8" s="63" t="b">
         <v>0</v>
       </c>
-      <c r="L8" s="67"/>
+      <c r="L8" s="55"/>
     </row>
     <row r="9" spans="2:12" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="60"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="67"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="67"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="55"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="60"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="73" t="s">
+      <c r="B10" s="48"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="77">
+      <c r="E10" s="65">
         <f>'Procura em Estoque'!E16-('Procura em Estoque'!E16*'Procura em Estoque'!E12)</f>
         <v>220.24799999999999</v>
       </c>
-      <c r="F10" s="67"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="73" t="s">
+      <c r="F10" s="55"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="K10" s="77" t="b">
+      <c r="K10" s="65" t="b">
         <f>E8=1</f>
         <v>0</v>
       </c>
-      <c r="L10" s="67"/>
+      <c r="L10" s="55"/>
     </row>
     <row r="11" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="60"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="67"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="67"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="55"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="55"/>
     </row>
     <row r="12" spans="2:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="60"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="70"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="70"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="58"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="58"/>
     </row>
     <row r="13" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="93"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="93"/>
-      <c r="C16" s="93"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="79"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="93"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="94" t="str">
+      <c r="B17" s="79"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="90" t="str">
         <f>_xlfn.IFS(NOT(K6),"Cadastrar Comprador",K8,"Fechar Pedido",AND(K6,K10),"Oferecer Mais Produtos",TRUE,"Fechar Pedido")</f>
         <v>Fechar Pedido</v>
       </c>
-      <c r="E17" s="95"/>
-      <c r="F17" s="93"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="79"/>
     </row>
     <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="97"/>
-      <c r="F18" s="93"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="79"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="93"/>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="93"/>
-      <c r="C20" s="93"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="93"/>
-      <c r="F20" s="93"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -10566,10 +10564,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="58"/>
+      <c r="B1" s="95"/>
       <c r="E1" s="34" t="s">
         <v>17</v>
       </c>
@@ -11038,18 +11036,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11071,6 +11069,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94D59180-AF5E-4D5F-B5F2-FD9983DB5A90}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B015A53-F126-4CCF-ABA9-FFC404E00010}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="44473e96-bad3-4ccd-b3db-2438e2abade5"/>
@@ -11084,12 +11090,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94D59180-AF5E-4D5F-B5F2-FD9983DB5A90}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>